<commit_message>
Changed create-excel-templates.js to use endpoints-spec.js vs the backend's *.api files.
</commit_message>
<xml_diff>
--- a/test/endpoints/templates/stats-endpoint.xlsx
+++ b/test/endpoints/templates/stats-endpoint.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -411,7 +411,6 @@
     <col min="6" max="6" customWidth="1" width="15"/>
     <col min="7" max="7" customWidth="1" width="15"/>
     <col min="8" max="8" customWidth="1" width="15"/>
-    <col min="9" max="9" customWidth="1" width="20"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -439,16 +438,13 @@
       <c r="H1" t="str">
         <v>tags</v>
       </c>
-      <c r="I1" t="str">
-        <v>param:unitName</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
         <v>stats - Basic Test</v>
       </c>
       <c r="B2" t="str">
-        <v>Test stats endpoint with valid parameters</v>
+        <v>Test GET /api/stats endpoint with valid parameters</v>
       </c>
       <c r="C2" t="str">
         <v>true</v>
@@ -468,13 +464,10 @@
       <c r="H2" t="str">
         <v>stats,functional</v>
       </c>
-      <c r="I2" t="str">
-        <v/>
-      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -498,130 +491,130 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>API Function:</v>
+        <v>HTTP Method:</v>
       </c>
       <c r="B3" t="str">
-        <v>stats</v>
+        <v>GET</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>File Path:</v>
+        <v>Path:</v>
       </c>
       <c r="B4" t="str">
-        <v>lux\stats.api</v>
+        <v>/api/stats</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v/>
+        <v>Description:</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Get system statistics</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Column Descriptions:</v>
+        <v/>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>test_name</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Unique identifier for the test</v>
+        <v>Column Descriptions:</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>description</v>
+        <v>test_name</v>
       </c>
       <c r="B8" t="str">
-        <v>Human-readable description of what the test does</v>
+        <v>Unique identifier for the test</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>enabled</v>
+        <v>description</v>
       </c>
       <c r="B9" t="str">
-        <v>Whether to run this test (true/false)</v>
+        <v>Human-readable description of what the test does</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>expected_status</v>
+        <v>enabled</v>
       </c>
       <c r="B10" t="str">
-        <v>Expected HTTP status code (200, 404, etc.)</v>
+        <v>Whether to run this test (true/false)</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>timeout_ms</v>
+        <v>expected_status</v>
       </c>
       <c r="B11" t="str">
-        <v>Request timeout in milliseconds</v>
+        <v>Expected HTTP status code (200, 404, etc.)</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>max_response_time</v>
+        <v>timeout_ms</v>
       </c>
       <c r="B12" t="str">
-        <v>Maximum acceptable response time in ms</v>
+        <v>Request timeout in milliseconds</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>delay_after_ms</v>
+        <v>max_response_time</v>
       </c>
       <c r="B13" t="str">
-        <v>Delay after test completion in ms</v>
+        <v>Maximum acceptable response time in ms</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>tags</v>
+        <v>delay_after_ms</v>
       </c>
       <c r="B14" t="str">
-        <v>Comma-separated tags for filtering tests</v>
+        <v>Delay after test completion in ms</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v/>
+        <v>tags</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Comma-separated tags for filtering tests</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>Parameter Descriptions:</v>
+        <v/>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>param:unitName</v>
-      </c>
-      <c r="B17" t="str">
-        <v>Unit name for multi-tenant deployments (string) (optional)</v>
+        <v/>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v/>
+        <v>Endpoint-Specific Notes:</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>Endpoint-Specific Notes:</v>
+        <v>• Method: GET</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>• Function: stats</v>
+        <v>• Path: /api/stats</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>• Optional parameters: unitName</v>
+        <v>• Description: Get system statistics</v>
       </c>
     </row>
   </sheetData>

</xml_diff>